<commit_message>
Actualizar precios desde Excel
</commit_message>
<xml_diff>
--- a/src/PreciosP.xlsx
+++ b/src/PreciosP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro\calculadora-energia\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7EF2E851-EB42-4707-9FC3-B39CB396D686}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74D57247-67D6-4103-AEC4-12596A21FFF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="490" windowWidth="19420" windowHeight="9700" xr2:uid="{01D25416-3606-4CF3-ADEB-58FCB3C46A56}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{01D25416-3606-4CF3-ADEB-58FCB3C46A56}"/>
   </bookViews>
   <sheets>
     <sheet name="3.0TD COMP" sheetId="2" r:id="rId1"/>
@@ -1007,29 +1007,51 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="13" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="13" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1043,57 +1065,35 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="166" fontId="13" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="13" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1145,10 +1145,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1451,7 +1447,7 @@
   <dimension ref="A1:AA52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1510,22 +1506,22 @@
         <v>0.02</v>
       </c>
       <c r="J2" s="2">
-        <v>7.0000000000000007E-2</v>
+        <v>4.4200000000000003E-2</v>
       </c>
       <c r="K2" s="2">
         <v>4.3700000000000003E-2</v>
       </c>
       <c r="L2" s="2">
         <f t="shared" ref="L2:L7" si="1">SUM(I2:K2)</f>
-        <v>0.13370000000000001</v>
+        <v>0.10790000000000001</v>
       </c>
       <c r="M2" s="2">
         <f t="shared" ref="M2:M7" si="2">L2*5%</f>
-        <v>6.6850000000000008E-3</v>
+        <v>5.3950000000000005E-3</v>
       </c>
       <c r="N2" s="3">
         <f t="shared" ref="N2:N7" si="3">L2+M2</f>
-        <v>0.14038500000000001</v>
+        <v>0.11329500000000001</v>
       </c>
       <c r="Q2" s="33">
         <v>4.3700000000000003E-2</v>
@@ -1813,20 +1809,20 @@
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="C9" s="60" t="s">
+      <c r="C9" s="80" t="s">
         <v>56</v>
       </c>
-      <c r="D9" s="60"/>
-      <c r="E9" s="60"/>
-      <c r="F9" s="60"/>
-      <c r="G9" s="60"/>
-      <c r="H9" s="60"/>
-      <c r="I9" s="60"/>
-      <c r="J9" s="60"/>
-      <c r="K9" s="60"/>
-      <c r="L9" s="60"/>
-      <c r="M9" s="60"/>
-      <c r="N9" s="60"/>
+      <c r="D9" s="80"/>
+      <c r="E9" s="80"/>
+      <c r="F9" s="80"/>
+      <c r="G9" s="80"/>
+      <c r="H9" s="80"/>
+      <c r="I9" s="80"/>
+      <c r="J9" s="80"/>
+      <c r="K9" s="80"/>
+      <c r="L9" s="80"/>
+      <c r="M9" s="80"/>
+      <c r="N9" s="80"/>
     </row>
     <row r="10" spans="1:22" ht="87" x14ac:dyDescent="0.35">
       <c r="C10" s="38" t="s">
@@ -1874,13 +1870,13 @@
       <c r="E11" s="40"/>
       <c r="F11" s="41">
         <f t="shared" ref="F11:F16" si="5">N2</f>
-        <v>0.14038500000000001</v>
+        <v>0.11329500000000001</v>
       </c>
       <c r="G11" s="43">
         <f t="shared" ref="G11:G16" si="6">E11*F11</f>
         <v>0</v>
       </c>
-      <c r="H11" s="61">
+      <c r="H11" s="81">
         <f>C17-G17</f>
         <v>433.70803999999998</v>
       </c>
@@ -1898,7 +1894,7 @@
         <v>338.67500000000001</v>
       </c>
       <c r="M11" s="40"/>
-      <c r="N11" s="64">
+      <c r="N11" s="84">
         <f>M17-L17</f>
         <v>2.0255999999999403</v>
       </c>
@@ -1917,7 +1913,7 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="H12" s="62"/>
+      <c r="H12" s="82"/>
       <c r="I12" s="42">
         <v>2.6599999999999999E-2</v>
       </c>
@@ -1932,7 +1928,7 @@
         <v>206.14999999999998</v>
       </c>
       <c r="M12" s="40"/>
-      <c r="N12" s="65"/>
+      <c r="N12" s="85"/>
     </row>
     <row r="13" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C13" s="40"/>
@@ -1948,7 +1944,7 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="H13" s="62"/>
+      <c r="H13" s="82"/>
       <c r="I13" s="42">
         <v>1.06E-2</v>
       </c>
@@ -1963,7 +1959,7 @@
         <v>82.149999999999991</v>
       </c>
       <c r="M13" s="40"/>
-      <c r="N13" s="65"/>
+      <c r="N13" s="85"/>
     </row>
     <row r="14" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C14" s="40"/>
@@ -1981,7 +1977,7 @@
         <f t="shared" si="6"/>
         <v>130.03746000000001</v>
       </c>
-      <c r="H14" s="62"/>
+      <c r="H14" s="82"/>
       <c r="I14" s="42">
         <v>1.15E-2</v>
       </c>
@@ -1996,7 +1992,7 @@
         <v>89.125</v>
       </c>
       <c r="M14" s="40"/>
-      <c r="N14" s="65"/>
+      <c r="N14" s="85"/>
     </row>
     <row r="15" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C15" s="40"/>
@@ -2014,7 +2010,7 @@
         <f t="shared" si="6"/>
         <v>90.735120000000023</v>
       </c>
-      <c r="H15" s="62"/>
+      <c r="H15" s="82"/>
       <c r="I15" s="42">
         <v>6.4000000000000003E-3</v>
       </c>
@@ -2029,7 +2025,7 @@
         <v>49.6</v>
       </c>
       <c r="M15" s="40"/>
-      <c r="N15" s="65"/>
+      <c r="N15" s="85"/>
     </row>
     <row r="16" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C16" s="40" t="s">
@@ -2049,7 +2045,7 @@
         <f t="shared" si="6"/>
         <v>89.749380000000016</v>
       </c>
-      <c r="H16" s="62"/>
+      <c r="H16" s="82"/>
       <c r="I16" s="42">
         <v>4.4000000000000003E-3</v>
       </c>
@@ -2064,7 +2060,7 @@
         <v>54.014400000000002</v>
       </c>
       <c r="M16" s="40"/>
-      <c r="N16" s="65"/>
+      <c r="N16" s="85"/>
     </row>
     <row r="17" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C17" s="45">
@@ -2077,7 +2073,7 @@
         <f>SUM(G12:G16)</f>
         <v>310.52196000000004</v>
       </c>
-      <c r="H17" s="63"/>
+      <c r="H17" s="83"/>
       <c r="I17" s="40"/>
       <c r="J17" s="40"/>
       <c r="K17" s="40"/>
@@ -2088,16 +2084,16 @@
       <c r="M17" s="48">
         <v>821.74</v>
       </c>
-      <c r="N17" s="66"/>
+      <c r="N17" s="86"/>
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="C18" s="71" t="s">
+      <c r="C18" s="78" t="s">
         <v>50</v>
       </c>
-      <c r="D18" s="71"/>
-      <c r="E18" s="71"/>
-      <c r="F18" s="71"/>
-      <c r="G18" s="71"/>
+      <c r="D18" s="78"/>
+      <c r="E18" s="78"/>
+      <c r="F18" s="78"/>
+      <c r="G18" s="78"/>
       <c r="H18" s="37">
         <f>H11*3</f>
         <v>1301.1241199999999</v>
@@ -2110,13 +2106,13 @@
       <c r="N18" s="47"/>
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="C19" s="72" t="s">
+      <c r="C19" s="79" t="s">
         <v>51</v>
       </c>
-      <c r="D19" s="72"/>
-      <c r="E19" s="72"/>
-      <c r="F19" s="72"/>
-      <c r="G19" s="72"/>
+      <c r="D19" s="79"/>
+      <c r="E19" s="79"/>
+      <c r="F19" s="79"/>
+      <c r="G19" s="79"/>
       <c r="H19" s="37">
         <f>H18*0.75</f>
         <v>975.84308999999996</v>
@@ -2125,13 +2121,13 @@
       <c r="N19" s="47"/>
     </row>
     <row r="20" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="C20" s="72" t="s">
+      <c r="C20" s="79" t="s">
         <v>52</v>
       </c>
-      <c r="D20" s="72"/>
-      <c r="E20" s="72"/>
-      <c r="F20" s="72"/>
-      <c r="G20" s="72"/>
+      <c r="D20" s="79"/>
+      <c r="E20" s="79"/>
+      <c r="F20" s="79"/>
+      <c r="G20" s="79"/>
       <c r="H20" s="37">
         <f>H18*0.7</f>
         <v>910.78688399999987</v>
@@ -2140,13 +2136,13 @@
       <c r="N20" s="47"/>
     </row>
     <row r="21" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="C21" s="67" t="s">
+      <c r="C21" s="77" t="s">
         <v>53</v>
       </c>
-      <c r="D21" s="67"/>
-      <c r="E21" s="67"/>
-      <c r="F21" s="67"/>
-      <c r="G21" s="67"/>
+      <c r="D21" s="77"/>
+      <c r="E21" s="77"/>
+      <c r="F21" s="77"/>
+      <c r="G21" s="77"/>
       <c r="H21" s="46">
         <f>SUM(H18:H20)</f>
         <v>3187.7540939999999</v>
@@ -2155,13 +2151,13 @@
       <c r="N21" s="47"/>
     </row>
     <row r="22" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="C22" s="67" t="s">
+      <c r="C22" s="77" t="s">
         <v>54</v>
       </c>
-      <c r="D22" s="67"/>
-      <c r="E22" s="67"/>
-      <c r="F22" s="67"/>
-      <c r="G22" s="67"/>
+      <c r="D22" s="77"/>
+      <c r="E22" s="77"/>
+      <c r="F22" s="77"/>
+      <c r="G22" s="77"/>
       <c r="H22" s="46">
         <f>(H11*12)*0.85</f>
         <v>4423.8220080000001</v>
@@ -2170,13 +2166,13 @@
       <c r="N22" s="47"/>
     </row>
     <row r="23" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="C23" s="67" t="s">
+      <c r="C23" s="77" t="s">
         <v>55</v>
       </c>
-      <c r="D23" s="67"/>
-      <c r="E23" s="67"/>
-      <c r="F23" s="67"/>
-      <c r="G23" s="67"/>
+      <c r="D23" s="77"/>
+      <c r="E23" s="77"/>
+      <c r="F23" s="77"/>
+      <c r="G23" s="77"/>
       <c r="H23" s="46">
         <f>H11*12</f>
         <v>5204.4964799999998</v>
@@ -2213,7 +2209,7 @@
       </c>
     </row>
     <row r="29" spans="1:27" s="6" customFormat="1" ht="28.5" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A29" s="68" t="s">
+      <c r="A29" s="74" t="s">
         <v>6</v>
       </c>
       <c r="B29" s="4"/>
@@ -2254,7 +2250,7 @@
       <c r="AA29" s="5"/>
     </row>
     <row r="30" spans="1:27" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="69"/>
+      <c r="A30" s="75"/>
       <c r="B30" s="7" t="s">
         <v>8</v>
       </c>
@@ -2277,7 +2273,7 @@
       </c>
     </row>
     <row r="31" spans="1:27" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="69"/>
+      <c r="A31" s="75"/>
       <c r="B31" s="7" t="s">
         <v>11</v>
       </c>
@@ -2320,7 +2316,7 @@
       <c r="O31" s="58"/>
     </row>
     <row r="32" spans="1:27" s="6" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="69"/>
+      <c r="A32" s="75"/>
       <c r="B32" s="7" t="s">
         <v>16</v>
       </c>
@@ -2363,7 +2359,7 @@
       <c r="O32" s="58"/>
     </row>
     <row r="33" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="69"/>
+      <c r="A33" s="75"/>
       <c r="B33" s="12" t="s">
         <v>29</v>
       </c>
@@ -2382,7 +2378,7 @@
       <c r="O33" s="58"/>
     </row>
     <row r="34" spans="1:27" s="6" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="69"/>
+      <c r="A34" s="75"/>
       <c r="B34" s="13" t="s">
         <v>30</v>
       </c>
@@ -2401,7 +2397,7 @@
       <c r="O34" s="58"/>
     </row>
     <row r="35" spans="1:27" s="6" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="69"/>
+      <c r="A35" s="75"/>
       <c r="B35" s="13" t="s">
         <v>31</v>
       </c>
@@ -2420,7 +2416,7 @@
       <c r="O35" s="58"/>
     </row>
     <row r="36" spans="1:27" s="6" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="69"/>
+      <c r="A36" s="75"/>
       <c r="B36" s="13" t="s">
         <v>32</v>
       </c>
@@ -2439,7 +2435,7 @@
       <c r="O36" s="58"/>
     </row>
     <row r="37" spans="1:27" s="6" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="69"/>
+      <c r="A37" s="75"/>
       <c r="B37" s="13" t="s">
         <v>33</v>
       </c>
@@ -2458,7 +2454,7 @@
       <c r="O37" s="58"/>
     </row>
     <row r="38" spans="1:27" s="6" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="69"/>
+      <c r="A38" s="75"/>
       <c r="B38" s="13" t="s">
         <v>34</v>
       </c>
@@ -2477,7 +2473,7 @@
       <c r="O38" s="58"/>
     </row>
     <row r="39" spans="1:27" s="6" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="70"/>
+      <c r="A39" s="76"/>
       <c r="B39" s="13" t="s">
         <v>35</v>
       </c>
@@ -2496,25 +2492,25 @@
       <c r="O39" s="58"/>
     </row>
     <row r="42" spans="1:27" s="6" customFormat="1" ht="28.5" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A42" s="75" t="s">
+      <c r="A42" s="62" t="s">
         <v>6</v>
       </c>
       <c r="B42" s="5"/>
-      <c r="C42" s="77" t="s">
+      <c r="C42" s="64" t="s">
         <v>36</v>
       </c>
-      <c r="D42" s="78"/>
-      <c r="E42" s="78"/>
-      <c r="F42" s="78"/>
-      <c r="G42" s="78"/>
-      <c r="H42" s="78"/>
-      <c r="I42" s="78"/>
-      <c r="J42" s="78"/>
-      <c r="K42" s="78"/>
-      <c r="L42" s="78"/>
-      <c r="M42" s="78"/>
-      <c r="N42" s="78"/>
-      <c r="O42" s="78"/>
+      <c r="D42" s="65"/>
+      <c r="E42" s="65"/>
+      <c r="F42" s="65"/>
+      <c r="G42" s="65"/>
+      <c r="H42" s="65"/>
+      <c r="I42" s="65"/>
+      <c r="J42" s="65"/>
+      <c r="K42" s="65"/>
+      <c r="L42" s="65"/>
+      <c r="M42" s="65"/>
+      <c r="N42" s="65"/>
+      <c r="O42" s="65"/>
       <c r="P42" s="5"/>
       <c r="Q42" s="5"/>
       <c r="R42" s="5"/>
@@ -2529,30 +2525,30 @@
       <c r="AA42" s="5"/>
     </row>
     <row r="43" spans="1:27" s="6" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="75"/>
+      <c r="A43" s="62"/>
       <c r="B43" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="C43" s="79" t="s">
+      <c r="C43" s="66" t="s">
         <v>9</v>
       </c>
-      <c r="D43" s="80"/>
-      <c r="E43" s="80"/>
-      <c r="F43" s="80"/>
-      <c r="G43" s="80"/>
-      <c r="H43" s="80"/>
-      <c r="I43" s="80"/>
-      <c r="J43" s="80"/>
-      <c r="K43" s="80"/>
-      <c r="L43" s="80"/>
-      <c r="M43" s="80"/>
-      <c r="N43" s="80"/>
-      <c r="O43" s="81" t="s">
+      <c r="D43" s="67"/>
+      <c r="E43" s="67"/>
+      <c r="F43" s="67"/>
+      <c r="G43" s="67"/>
+      <c r="H43" s="67"/>
+      <c r="I43" s="67"/>
+      <c r="J43" s="67"/>
+      <c r="K43" s="67"/>
+      <c r="L43" s="67"/>
+      <c r="M43" s="67"/>
+      <c r="N43" s="67"/>
+      <c r="O43" s="68" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="44" spans="1:27" s="6" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="75"/>
+      <c r="A44" s="62"/>
       <c r="B44" s="18" t="s">
         <v>11</v>
       </c>
@@ -2592,72 +2588,72 @@
       <c r="N44" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="O44" s="82"/>
+      <c r="O44" s="69"/>
     </row>
     <row r="45" spans="1:27" s="6" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="75"/>
+      <c r="A45" s="62"/>
       <c r="B45" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="C45" s="85" t="s">
+      <c r="C45" s="72" t="s">
         <v>17</v>
       </c>
-      <c r="D45" s="85" t="s">
+      <c r="D45" s="72" t="s">
         <v>18</v>
       </c>
-      <c r="E45" s="85" t="s">
+      <c r="E45" s="72" t="s">
         <v>19</v>
       </c>
-      <c r="F45" s="85" t="s">
+      <c r="F45" s="72" t="s">
         <v>20</v>
       </c>
-      <c r="G45" s="85" t="s">
+      <c r="G45" s="72" t="s">
         <v>21</v>
       </c>
-      <c r="H45" s="85" t="s">
+      <c r="H45" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="I45" s="85" t="s">
+      <c r="I45" s="72" t="s">
         <v>23</v>
       </c>
-      <c r="J45" s="85" t="s">
+      <c r="J45" s="72" t="s">
         <v>24</v>
       </c>
-      <c r="K45" s="85" t="s">
+      <c r="K45" s="72" t="s">
         <v>25</v>
       </c>
-      <c r="L45" s="85" t="s">
+      <c r="L45" s="72" t="s">
         <v>26</v>
       </c>
-      <c r="M45" s="85" t="s">
+      <c r="M45" s="72" t="s">
         <v>27</v>
       </c>
-      <c r="N45" s="73" t="s">
+      <c r="N45" s="60" t="s">
         <v>28</v>
       </c>
-      <c r="O45" s="82"/>
+      <c r="O45" s="69"/>
     </row>
     <row r="46" spans="1:27" s="6" customFormat="1" ht="23.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="75"/>
+      <c r="A46" s="62"/>
       <c r="B46" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="C46" s="86"/>
-      <c r="D46" s="86"/>
-      <c r="E46" s="86"/>
-      <c r="F46" s="86"/>
-      <c r="G46" s="86"/>
-      <c r="H46" s="86"/>
-      <c r="I46" s="86"/>
-      <c r="J46" s="86"/>
-      <c r="K46" s="86"/>
-      <c r="L46" s="86"/>
-      <c r="M46" s="86"/>
-      <c r="N46" s="74"/>
-      <c r="O46" s="82"/>
+      <c r="C46" s="73"/>
+      <c r="D46" s="73"/>
+      <c r="E46" s="73"/>
+      <c r="F46" s="73"/>
+      <c r="G46" s="73"/>
+      <c r="H46" s="73"/>
+      <c r="I46" s="73"/>
+      <c r="J46" s="73"/>
+      <c r="K46" s="73"/>
+      <c r="L46" s="73"/>
+      <c r="M46" s="73"/>
+      <c r="N46" s="61"/>
+      <c r="O46" s="69"/>
     </row>
     <row r="47" spans="1:27" s="6" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="75"/>
+      <c r="A47" s="62"/>
       <c r="B47" s="25" t="s">
         <v>30</v>
       </c>
@@ -2673,10 +2669,10 @@
       <c r="L47" s="16"/>
       <c r="M47" s="15"/>
       <c r="N47" s="15"/>
-      <c r="O47" s="83"/>
+      <c r="O47" s="70"/>
     </row>
     <row r="48" spans="1:27" s="6" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="75"/>
+      <c r="A48" s="62"/>
       <c r="B48" s="26" t="s">
         <v>31</v>
       </c>
@@ -2692,10 +2688,10 @@
       <c r="L48" s="15"/>
       <c r="M48" s="16"/>
       <c r="N48" s="16"/>
-      <c r="O48" s="83"/>
+      <c r="O48" s="70"/>
     </row>
     <row r="49" spans="1:15" s="6" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="75"/>
+      <c r="A49" s="62"/>
       <c r="B49" s="27" t="s">
         <v>32</v>
       </c>
@@ -2711,10 +2707,10 @@
       <c r="L49" s="16"/>
       <c r="M49" s="16"/>
       <c r="N49" s="16"/>
-      <c r="O49" s="83"/>
+      <c r="O49" s="70"/>
     </row>
     <row r="50" spans="1:15" s="6" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="75"/>
+      <c r="A50" s="62"/>
       <c r="B50" s="28" t="s">
         <v>33</v>
       </c>
@@ -2730,10 +2726,10 @@
       <c r="L50" s="15"/>
       <c r="M50" s="15"/>
       <c r="N50" s="15"/>
-      <c r="O50" s="83"/>
+      <c r="O50" s="70"/>
     </row>
     <row r="51" spans="1:15" s="6" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="75"/>
+      <c r="A51" s="62"/>
       <c r="B51" s="26" t="s">
         <v>34</v>
       </c>
@@ -2749,10 +2745,10 @@
       <c r="L51" s="15"/>
       <c r="M51" s="15"/>
       <c r="N51" s="15"/>
-      <c r="O51" s="83"/>
+      <c r="O51" s="70"/>
     </row>
     <row r="52" spans="1:15" s="6" customFormat="1" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A52" s="76"/>
+      <c r="A52" s="63"/>
       <c r="B52" s="27" t="s">
         <v>35</v>
       </c>
@@ -2768,10 +2764,20 @@
       <c r="L52" s="16"/>
       <c r="M52" s="16"/>
       <c r="N52" s="16"/>
-      <c r="O52" s="84"/>
+      <c r="O52" s="71"/>
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="C9:N9"/>
+    <mergeCell ref="H11:H17"/>
+    <mergeCell ref="N11:N17"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="A29:A39"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
     <mergeCell ref="N45:N46"/>
     <mergeCell ref="A42:A52"/>
     <mergeCell ref="C42:O42"/>
@@ -2788,16 +2794,6 @@
     <mergeCell ref="K45:K46"/>
     <mergeCell ref="L45:L46"/>
     <mergeCell ref="M45:M46"/>
-    <mergeCell ref="A29:A39"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C9:N9"/>
-    <mergeCell ref="H11:H17"/>
-    <mergeCell ref="N11:N17"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3082,7 +3078,7 @@
         <v>60.489640006900004</v>
       </c>
       <c r="N11" s="40"/>
-      <c r="O11" s="64">
+      <c r="O11" s="84">
         <f>N17-M17</f>
         <v>20.038733764899973</v>
       </c>
@@ -3119,7 +3115,7 @@
         <v>30.272243851199999</v>
       </c>
       <c r="N12" s="40"/>
-      <c r="O12" s="65"/>
+      <c r="O12" s="85"/>
     </row>
     <row r="13" spans="3:15" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C13" s="40"/>
@@ -3151,7 +3147,7 @@
         <v>21.996228436000003</v>
       </c>
       <c r="N13" s="40"/>
-      <c r="O13" s="65"/>
+      <c r="O13" s="85"/>
     </row>
     <row r="14" spans="3:15" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C14" s="40"/>
@@ -3183,7 +3179,7 @@
         <v>21.996228436000003</v>
       </c>
       <c r="N14" s="40"/>
-      <c r="O14" s="65"/>
+      <c r="O14" s="85"/>
     </row>
     <row r="15" spans="3:15" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C15" s="40"/>
@@ -3215,7 +3211,7 @@
         <v>21.996228436000003</v>
       </c>
       <c r="N15" s="40"/>
-      <c r="O15" s="65"/>
+      <c r="O15" s="85"/>
     </row>
     <row r="16" spans="3:15" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C16" s="40" t="s">
@@ -3251,7 +3247,7 @@
         <v>13.220697069000002</v>
       </c>
       <c r="N16" s="40"/>
-      <c r="O16" s="65"/>
+      <c r="O16" s="85"/>
     </row>
     <row r="17" spans="3:15" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C17" s="45">
@@ -3278,81 +3274,81 @@
         <f>93.14+48.78+21.22+16.73+6.25+3.89</f>
         <v>190.01</v>
       </c>
-      <c r="O17" s="66"/>
+      <c r="O17" s="86"/>
     </row>
     <row r="18" spans="3:15" x14ac:dyDescent="0.35">
-      <c r="C18" s="71" t="s">
+      <c r="C18" s="78" t="s">
         <v>50</v>
       </c>
-      <c r="D18" s="71"/>
-      <c r="E18" s="71"/>
-      <c r="F18" s="71"/>
-      <c r="G18" s="71"/>
+      <c r="D18" s="78"/>
+      <c r="E18" s="78"/>
+      <c r="F18" s="78"/>
+      <c r="G18" s="78"/>
       <c r="H18" s="37">
         <f>H11*3+O11*3</f>
         <v>1397.7352039346997</v>
       </c>
     </row>
     <row r="19" spans="3:15" x14ac:dyDescent="0.35">
-      <c r="C19" s="72" t="s">
+      <c r="C19" s="79" t="s">
         <v>51</v>
       </c>
-      <c r="D19" s="72"/>
-      <c r="E19" s="72"/>
-      <c r="F19" s="72"/>
-      <c r="G19" s="72"/>
+      <c r="D19" s="79"/>
+      <c r="E19" s="79"/>
+      <c r="F19" s="79"/>
+      <c r="G19" s="79"/>
       <c r="H19" s="37">
         <f>H18*0.75</f>
         <v>1048.3014029510248</v>
       </c>
     </row>
     <row r="20" spans="3:15" x14ac:dyDescent="0.35">
-      <c r="C20" s="72" t="s">
+      <c r="C20" s="79" t="s">
         <v>52</v>
       </c>
-      <c r="D20" s="72"/>
-      <c r="E20" s="72"/>
-      <c r="F20" s="72"/>
-      <c r="G20" s="72"/>
+      <c r="D20" s="79"/>
+      <c r="E20" s="79"/>
+      <c r="F20" s="79"/>
+      <c r="G20" s="79"/>
       <c r="H20" s="37">
         <f>H18*0.7</f>
         <v>978.41464275428973</v>
       </c>
     </row>
     <row r="21" spans="3:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="C21" s="67" t="s">
+      <c r="C21" s="77" t="s">
         <v>53</v>
       </c>
-      <c r="D21" s="67"/>
-      <c r="E21" s="67"/>
-      <c r="F21" s="67"/>
-      <c r="G21" s="67"/>
+      <c r="D21" s="77"/>
+      <c r="E21" s="77"/>
+      <c r="F21" s="77"/>
+      <c r="G21" s="77"/>
       <c r="H21" s="46">
         <f>SUM(H18:H20)</f>
         <v>3424.4512496400143</v>
       </c>
     </row>
     <row r="22" spans="3:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="C22" s="67" t="s">
+      <c r="C22" s="77" t="s">
         <v>54</v>
       </c>
-      <c r="D22" s="67"/>
-      <c r="E22" s="67"/>
-      <c r="F22" s="67"/>
-      <c r="G22" s="67"/>
+      <c r="D22" s="77"/>
+      <c r="E22" s="77"/>
+      <c r="F22" s="77"/>
+      <c r="G22" s="77"/>
       <c r="H22" s="46">
         <f>(H11*12)*0.85</f>
         <v>4547.9046089759986</v>
       </c>
     </row>
     <row r="23" spans="3:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="C23" s="67" t="s">
+      <c r="C23" s="77" t="s">
         <v>55</v>
       </c>
-      <c r="D23" s="67"/>
-      <c r="E23" s="67"/>
-      <c r="F23" s="67"/>
-      <c r="G23" s="67"/>
+      <c r="D23" s="77"/>
+      <c r="E23" s="77"/>
+      <c r="F23" s="77"/>
+      <c r="G23" s="77"/>
       <c r="H23" s="46">
         <f>H11*12</f>
         <v>5350.4760105599989</v>

</xml_diff>

<commit_message>
Forzar actualización de precios
</commit_message>
<xml_diff>
--- a/src/PreciosP.xlsx
+++ b/src/PreciosP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro\calculadora-energia\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77500343-9F60-447A-9150-3E6B15642661}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6BADEAC-BCC0-415D-9A0A-877F834A0D11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{01D25416-3606-4CF3-ADEB-58FCB3C46A56}"/>
   </bookViews>
@@ -1007,6 +1007,48 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="13" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="13" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1052,48 +1094,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="13" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="13" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1506,22 +1506,22 @@
         <v>0.02</v>
       </c>
       <c r="J2" s="2">
-        <v>4.4200000000000003E-2</v>
+        <v>4.4200999999999997E-2</v>
       </c>
       <c r="K2" s="2">
         <v>4.3700000000000003E-2</v>
       </c>
       <c r="L2" s="2">
         <f t="shared" ref="L2:L7" si="1">SUM(I2:K2)</f>
-        <v>0.10790000000000001</v>
+        <v>0.107901</v>
       </c>
       <c r="M2" s="2">
         <f t="shared" ref="M2:M7" si="2">L2*5%</f>
-        <v>5.3950000000000005E-3</v>
+        <v>5.3950500000000002E-3</v>
       </c>
       <c r="N2" s="3">
         <f t="shared" ref="N2:N7" si="3">L2+M2</f>
-        <v>0.11329500000000001</v>
+        <v>0.11329605</v>
       </c>
       <c r="Q2" s="33">
         <v>4.3700000000000003E-2</v>
@@ -1809,20 +1809,20 @@
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="C9" s="80" t="s">
+      <c r="C9" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="D9" s="80"/>
-      <c r="E9" s="80"/>
-      <c r="F9" s="80"/>
-      <c r="G9" s="80"/>
-      <c r="H9" s="80"/>
-      <c r="I9" s="80"/>
-      <c r="J9" s="80"/>
-      <c r="K9" s="80"/>
-      <c r="L9" s="80"/>
-      <c r="M9" s="80"/>
-      <c r="N9" s="80"/>
+      <c r="D9" s="60"/>
+      <c r="E9" s="60"/>
+      <c r="F9" s="60"/>
+      <c r="G9" s="60"/>
+      <c r="H9" s="60"/>
+      <c r="I9" s="60"/>
+      <c r="J9" s="60"/>
+      <c r="K9" s="60"/>
+      <c r="L9" s="60"/>
+      <c r="M9" s="60"/>
+      <c r="N9" s="60"/>
     </row>
     <row r="10" spans="1:22" ht="87" x14ac:dyDescent="0.35">
       <c r="C10" s="38" t="s">
@@ -1870,13 +1870,13 @@
       <c r="E11" s="40"/>
       <c r="F11" s="41">
         <f t="shared" ref="F11:F16" si="5">N2</f>
-        <v>0.11329500000000001</v>
+        <v>0.11329605</v>
       </c>
       <c r="G11" s="43">
         <f t="shared" ref="G11:G16" si="6">E11*F11</f>
         <v>0</v>
       </c>
-      <c r="H11" s="81">
+      <c r="H11" s="61">
         <f>C17-G17</f>
         <v>433.70803999999998</v>
       </c>
@@ -1894,7 +1894,7 @@
         <v>338.67500000000001</v>
       </c>
       <c r="M11" s="40"/>
-      <c r="N11" s="84">
+      <c r="N11" s="64">
         <f>M17-L17</f>
         <v>2.0255999999999403</v>
       </c>
@@ -1913,7 +1913,7 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="H12" s="82"/>
+      <c r="H12" s="62"/>
       <c r="I12" s="42">
         <v>2.6599999999999999E-2</v>
       </c>
@@ -1928,7 +1928,7 @@
         <v>206.14999999999998</v>
       </c>
       <c r="M12" s="40"/>
-      <c r="N12" s="85"/>
+      <c r="N12" s="65"/>
     </row>
     <row r="13" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C13" s="40"/>
@@ -1944,7 +1944,7 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="H13" s="82"/>
+      <c r="H13" s="62"/>
       <c r="I13" s="42">
         <v>1.06E-2</v>
       </c>
@@ -1959,7 +1959,7 @@
         <v>82.149999999999991</v>
       </c>
       <c r="M13" s="40"/>
-      <c r="N13" s="85"/>
+      <c r="N13" s="65"/>
     </row>
     <row r="14" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C14" s="40"/>
@@ -1977,7 +1977,7 @@
         <f t="shared" si="6"/>
         <v>130.03746000000001</v>
       </c>
-      <c r="H14" s="82"/>
+      <c r="H14" s="62"/>
       <c r="I14" s="42">
         <v>1.15E-2</v>
       </c>
@@ -1992,7 +1992,7 @@
         <v>89.125</v>
       </c>
       <c r="M14" s="40"/>
-      <c r="N14" s="85"/>
+      <c r="N14" s="65"/>
     </row>
     <row r="15" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C15" s="40"/>
@@ -2010,7 +2010,7 @@
         <f t="shared" si="6"/>
         <v>90.735120000000023</v>
       </c>
-      <c r="H15" s="82"/>
+      <c r="H15" s="62"/>
       <c r="I15" s="42">
         <v>6.4000000000000003E-3</v>
       </c>
@@ -2025,7 +2025,7 @@
         <v>49.6</v>
       </c>
       <c r="M15" s="40"/>
-      <c r="N15" s="85"/>
+      <c r="N15" s="65"/>
     </row>
     <row r="16" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C16" s="40" t="s">
@@ -2045,7 +2045,7 @@
         <f t="shared" si="6"/>
         <v>89.749380000000016</v>
       </c>
-      <c r="H16" s="82"/>
+      <c r="H16" s="62"/>
       <c r="I16" s="42">
         <v>4.4000000000000003E-3</v>
       </c>
@@ -2060,7 +2060,7 @@
         <v>54.014400000000002</v>
       </c>
       <c r="M16" s="40"/>
-      <c r="N16" s="85"/>
+      <c r="N16" s="65"/>
     </row>
     <row r="17" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C17" s="45">
@@ -2073,7 +2073,7 @@
         <f>SUM(G12:G16)</f>
         <v>310.52196000000004</v>
       </c>
-      <c r="H17" s="83"/>
+      <c r="H17" s="63"/>
       <c r="I17" s="40"/>
       <c r="J17" s="40"/>
       <c r="K17" s="40"/>
@@ -2084,16 +2084,16 @@
       <c r="M17" s="48">
         <v>821.74</v>
       </c>
-      <c r="N17" s="86"/>
+      <c r="N17" s="66"/>
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="C18" s="78" t="s">
+      <c r="C18" s="71" t="s">
         <v>50</v>
       </c>
-      <c r="D18" s="78"/>
-      <c r="E18" s="78"/>
-      <c r="F18" s="78"/>
-      <c r="G18" s="78"/>
+      <c r="D18" s="71"/>
+      <c r="E18" s="71"/>
+      <c r="F18" s="71"/>
+      <c r="G18" s="71"/>
       <c r="H18" s="37">
         <f>H11*3</f>
         <v>1301.1241199999999</v>
@@ -2106,13 +2106,13 @@
       <c r="N18" s="47"/>
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="C19" s="79" t="s">
+      <c r="C19" s="72" t="s">
         <v>51</v>
       </c>
-      <c r="D19" s="79"/>
-      <c r="E19" s="79"/>
-      <c r="F19" s="79"/>
-      <c r="G19" s="79"/>
+      <c r="D19" s="72"/>
+      <c r="E19" s="72"/>
+      <c r="F19" s="72"/>
+      <c r="G19" s="72"/>
       <c r="H19" s="37">
         <f>H18*0.75</f>
         <v>975.84308999999996</v>
@@ -2121,13 +2121,13 @@
       <c r="N19" s="47"/>
     </row>
     <row r="20" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="C20" s="79" t="s">
+      <c r="C20" s="72" t="s">
         <v>52</v>
       </c>
-      <c r="D20" s="79"/>
-      <c r="E20" s="79"/>
-      <c r="F20" s="79"/>
-      <c r="G20" s="79"/>
+      <c r="D20" s="72"/>
+      <c r="E20" s="72"/>
+      <c r="F20" s="72"/>
+      <c r="G20" s="72"/>
       <c r="H20" s="37">
         <f>H18*0.7</f>
         <v>910.78688399999987</v>
@@ -2136,13 +2136,13 @@
       <c r="N20" s="47"/>
     </row>
     <row r="21" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="C21" s="77" t="s">
+      <c r="C21" s="67" t="s">
         <v>53</v>
       </c>
-      <c r="D21" s="77"/>
-      <c r="E21" s="77"/>
-      <c r="F21" s="77"/>
-      <c r="G21" s="77"/>
+      <c r="D21" s="67"/>
+      <c r="E21" s="67"/>
+      <c r="F21" s="67"/>
+      <c r="G21" s="67"/>
       <c r="H21" s="46">
         <f>SUM(H18:H20)</f>
         <v>3187.7540939999999</v>
@@ -2151,13 +2151,13 @@
       <c r="N21" s="47"/>
     </row>
     <row r="22" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="C22" s="77" t="s">
+      <c r="C22" s="67" t="s">
         <v>54</v>
       </c>
-      <c r="D22" s="77"/>
-      <c r="E22" s="77"/>
-      <c r="F22" s="77"/>
-      <c r="G22" s="77"/>
+      <c r="D22" s="67"/>
+      <c r="E22" s="67"/>
+      <c r="F22" s="67"/>
+      <c r="G22" s="67"/>
       <c r="H22" s="46">
         <f>(H11*12)*0.85</f>
         <v>4423.8220080000001</v>
@@ -2166,13 +2166,13 @@
       <c r="N22" s="47"/>
     </row>
     <row r="23" spans="1:27" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="C23" s="77" t="s">
+      <c r="C23" s="67" t="s">
         <v>55</v>
       </c>
-      <c r="D23" s="77"/>
-      <c r="E23" s="77"/>
-      <c r="F23" s="77"/>
-      <c r="G23" s="77"/>
+      <c r="D23" s="67"/>
+      <c r="E23" s="67"/>
+      <c r="F23" s="67"/>
+      <c r="G23" s="67"/>
       <c r="H23" s="46">
         <f>H11*12</f>
         <v>5204.4964799999998</v>
@@ -2209,7 +2209,7 @@
       </c>
     </row>
     <row r="29" spans="1:27" s="6" customFormat="1" ht="28.5" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A29" s="74" t="s">
+      <c r="A29" s="68" t="s">
         <v>6</v>
       </c>
       <c r="B29" s="4"/>
@@ -2250,7 +2250,7 @@
       <c r="AA29" s="5"/>
     </row>
     <row r="30" spans="1:27" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="75"/>
+      <c r="A30" s="69"/>
       <c r="B30" s="7" t="s">
         <v>8</v>
       </c>
@@ -2273,7 +2273,7 @@
       </c>
     </row>
     <row r="31" spans="1:27" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="75"/>
+      <c r="A31" s="69"/>
       <c r="B31" s="7" t="s">
         <v>11</v>
       </c>
@@ -2316,7 +2316,7 @@
       <c r="O31" s="58"/>
     </row>
     <row r="32" spans="1:27" s="6" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="75"/>
+      <c r="A32" s="69"/>
       <c r="B32" s="7" t="s">
         <v>16</v>
       </c>
@@ -2359,7 +2359,7 @@
       <c r="O32" s="58"/>
     </row>
     <row r="33" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="75"/>
+      <c r="A33" s="69"/>
       <c r="B33" s="12" t="s">
         <v>29</v>
       </c>
@@ -2378,7 +2378,7 @@
       <c r="O33" s="58"/>
     </row>
     <row r="34" spans="1:27" s="6" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="75"/>
+      <c r="A34" s="69"/>
       <c r="B34" s="13" t="s">
         <v>30</v>
       </c>
@@ -2397,7 +2397,7 @@
       <c r="O34" s="58"/>
     </row>
     <row r="35" spans="1:27" s="6" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="75"/>
+      <c r="A35" s="69"/>
       <c r="B35" s="13" t="s">
         <v>31</v>
       </c>
@@ -2416,7 +2416,7 @@
       <c r="O35" s="58"/>
     </row>
     <row r="36" spans="1:27" s="6" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="75"/>
+      <c r="A36" s="69"/>
       <c r="B36" s="13" t="s">
         <v>32</v>
       </c>
@@ -2435,7 +2435,7 @@
       <c r="O36" s="58"/>
     </row>
     <row r="37" spans="1:27" s="6" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="75"/>
+      <c r="A37" s="69"/>
       <c r="B37" s="13" t="s">
         <v>33</v>
       </c>
@@ -2454,7 +2454,7 @@
       <c r="O37" s="58"/>
     </row>
     <row r="38" spans="1:27" s="6" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="75"/>
+      <c r="A38" s="69"/>
       <c r="B38" s="13" t="s">
         <v>34</v>
       </c>
@@ -2473,7 +2473,7 @@
       <c r="O38" s="58"/>
     </row>
     <row r="39" spans="1:27" s="6" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="76"/>
+      <c r="A39" s="70"/>
       <c r="B39" s="13" t="s">
         <v>35</v>
       </c>
@@ -2492,25 +2492,25 @@
       <c r="O39" s="58"/>
     </row>
     <row r="42" spans="1:27" s="6" customFormat="1" ht="28.5" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A42" s="62" t="s">
+      <c r="A42" s="75" t="s">
         <v>6</v>
       </c>
       <c r="B42" s="5"/>
-      <c r="C42" s="64" t="s">
+      <c r="C42" s="77" t="s">
         <v>36</v>
       </c>
-      <c r="D42" s="65"/>
-      <c r="E42" s="65"/>
-      <c r="F42" s="65"/>
-      <c r="G42" s="65"/>
-      <c r="H42" s="65"/>
-      <c r="I42" s="65"/>
-      <c r="J42" s="65"/>
-      <c r="K42" s="65"/>
-      <c r="L42" s="65"/>
-      <c r="M42" s="65"/>
-      <c r="N42" s="65"/>
-      <c r="O42" s="65"/>
+      <c r="D42" s="78"/>
+      <c r="E42" s="78"/>
+      <c r="F42" s="78"/>
+      <c r="G42" s="78"/>
+      <c r="H42" s="78"/>
+      <c r="I42" s="78"/>
+      <c r="J42" s="78"/>
+      <c r="K42" s="78"/>
+      <c r="L42" s="78"/>
+      <c r="M42" s="78"/>
+      <c r="N42" s="78"/>
+      <c r="O42" s="78"/>
       <c r="P42" s="5"/>
       <c r="Q42" s="5"/>
       <c r="R42" s="5"/>
@@ -2525,30 +2525,30 @@
       <c r="AA42" s="5"/>
     </row>
     <row r="43" spans="1:27" s="6" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="62"/>
+      <c r="A43" s="75"/>
       <c r="B43" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="C43" s="66" t="s">
+      <c r="C43" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="D43" s="67"/>
-      <c r="E43" s="67"/>
-      <c r="F43" s="67"/>
-      <c r="G43" s="67"/>
-      <c r="H43" s="67"/>
-      <c r="I43" s="67"/>
-      <c r="J43" s="67"/>
-      <c r="K43" s="67"/>
-      <c r="L43" s="67"/>
-      <c r="M43" s="67"/>
-      <c r="N43" s="67"/>
-      <c r="O43" s="68" t="s">
+      <c r="D43" s="80"/>
+      <c r="E43" s="80"/>
+      <c r="F43" s="80"/>
+      <c r="G43" s="80"/>
+      <c r="H43" s="80"/>
+      <c r="I43" s="80"/>
+      <c r="J43" s="80"/>
+      <c r="K43" s="80"/>
+      <c r="L43" s="80"/>
+      <c r="M43" s="80"/>
+      <c r="N43" s="80"/>
+      <c r="O43" s="81" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="44" spans="1:27" s="6" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="62"/>
+      <c r="A44" s="75"/>
       <c r="B44" s="18" t="s">
         <v>11</v>
       </c>
@@ -2588,72 +2588,72 @@
       <c r="N44" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="O44" s="69"/>
+      <c r="O44" s="82"/>
     </row>
     <row r="45" spans="1:27" s="6" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="62"/>
+      <c r="A45" s="75"/>
       <c r="B45" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="C45" s="72" t="s">
+      <c r="C45" s="85" t="s">
         <v>17</v>
       </c>
-      <c r="D45" s="72" t="s">
+      <c r="D45" s="85" t="s">
         <v>18</v>
       </c>
-      <c r="E45" s="72" t="s">
+      <c r="E45" s="85" t="s">
         <v>19</v>
       </c>
-      <c r="F45" s="72" t="s">
+      <c r="F45" s="85" t="s">
         <v>20</v>
       </c>
-      <c r="G45" s="72" t="s">
+      <c r="G45" s="85" t="s">
         <v>21</v>
       </c>
-      <c r="H45" s="72" t="s">
+      <c r="H45" s="85" t="s">
         <v>22</v>
       </c>
-      <c r="I45" s="72" t="s">
+      <c r="I45" s="85" t="s">
         <v>23</v>
       </c>
-      <c r="J45" s="72" t="s">
+      <c r="J45" s="85" t="s">
         <v>24</v>
       </c>
-      <c r="K45" s="72" t="s">
+      <c r="K45" s="85" t="s">
         <v>25</v>
       </c>
-      <c r="L45" s="72" t="s">
+      <c r="L45" s="85" t="s">
         <v>26</v>
       </c>
-      <c r="M45" s="72" t="s">
+      <c r="M45" s="85" t="s">
         <v>27</v>
       </c>
-      <c r="N45" s="60" t="s">
+      <c r="N45" s="73" t="s">
         <v>28</v>
       </c>
-      <c r="O45" s="69"/>
+      <c r="O45" s="82"/>
     </row>
     <row r="46" spans="1:27" s="6" customFormat="1" ht="23.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="62"/>
+      <c r="A46" s="75"/>
       <c r="B46" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="C46" s="73"/>
-      <c r="D46" s="73"/>
-      <c r="E46" s="73"/>
-      <c r="F46" s="73"/>
-      <c r="G46" s="73"/>
-      <c r="H46" s="73"/>
-      <c r="I46" s="73"/>
-      <c r="J46" s="73"/>
-      <c r="K46" s="73"/>
-      <c r="L46" s="73"/>
-      <c r="M46" s="73"/>
-      <c r="N46" s="61"/>
-      <c r="O46" s="69"/>
+      <c r="C46" s="86"/>
+      <c r="D46" s="86"/>
+      <c r="E46" s="86"/>
+      <c r="F46" s="86"/>
+      <c r="G46" s="86"/>
+      <c r="H46" s="86"/>
+      <c r="I46" s="86"/>
+      <c r="J46" s="86"/>
+      <c r="K46" s="86"/>
+      <c r="L46" s="86"/>
+      <c r="M46" s="86"/>
+      <c r="N46" s="74"/>
+      <c r="O46" s="82"/>
     </row>
     <row r="47" spans="1:27" s="6" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="62"/>
+      <c r="A47" s="75"/>
       <c r="B47" s="25" t="s">
         <v>30</v>
       </c>
@@ -2669,10 +2669,10 @@
       <c r="L47" s="16"/>
       <c r="M47" s="15"/>
       <c r="N47" s="15"/>
-      <c r="O47" s="70"/>
+      <c r="O47" s="83"/>
     </row>
     <row r="48" spans="1:27" s="6" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="62"/>
+      <c r="A48" s="75"/>
       <c r="B48" s="26" t="s">
         <v>31</v>
       </c>
@@ -2688,10 +2688,10 @@
       <c r="L48" s="15"/>
       <c r="M48" s="16"/>
       <c r="N48" s="16"/>
-      <c r="O48" s="70"/>
+      <c r="O48" s="83"/>
     </row>
     <row r="49" spans="1:15" s="6" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="62"/>
+      <c r="A49" s="75"/>
       <c r="B49" s="27" t="s">
         <v>32</v>
       </c>
@@ -2707,10 +2707,10 @@
       <c r="L49" s="16"/>
       <c r="M49" s="16"/>
       <c r="N49" s="16"/>
-      <c r="O49" s="70"/>
+      <c r="O49" s="83"/>
     </row>
     <row r="50" spans="1:15" s="6" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="62"/>
+      <c r="A50" s="75"/>
       <c r="B50" s="28" t="s">
         <v>33</v>
       </c>
@@ -2726,10 +2726,10 @@
       <c r="L50" s="15"/>
       <c r="M50" s="15"/>
       <c r="N50" s="15"/>
-      <c r="O50" s="70"/>
+      <c r="O50" s="83"/>
     </row>
     <row r="51" spans="1:15" s="6" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="62"/>
+      <c r="A51" s="75"/>
       <c r="B51" s="26" t="s">
         <v>34</v>
       </c>
@@ -2745,10 +2745,10 @@
       <c r="L51" s="15"/>
       <c r="M51" s="15"/>
       <c r="N51" s="15"/>
-      <c r="O51" s="70"/>
+      <c r="O51" s="83"/>
     </row>
     <row r="52" spans="1:15" s="6" customFormat="1" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A52" s="63"/>
+      <c r="A52" s="76"/>
       <c r="B52" s="27" t="s">
         <v>35</v>
       </c>
@@ -2764,20 +2764,10 @@
       <c r="L52" s="16"/>
       <c r="M52" s="16"/>
       <c r="N52" s="16"/>
-      <c r="O52" s="71"/>
+      <c r="O52" s="84"/>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="C9:N9"/>
-    <mergeCell ref="H11:H17"/>
-    <mergeCell ref="N11:N17"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="A29:A39"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
     <mergeCell ref="N45:N46"/>
     <mergeCell ref="A42:A52"/>
     <mergeCell ref="C42:O42"/>
@@ -2794,6 +2784,16 @@
     <mergeCell ref="K45:K46"/>
     <mergeCell ref="L45:L46"/>
     <mergeCell ref="M45:M46"/>
+    <mergeCell ref="A29:A39"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C9:N9"/>
+    <mergeCell ref="H11:H17"/>
+    <mergeCell ref="N11:N17"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="C22:G22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3078,7 +3078,7 @@
         <v>60.489640006900004</v>
       </c>
       <c r="N11" s="40"/>
-      <c r="O11" s="84">
+      <c r="O11" s="64">
         <f>N17-M17</f>
         <v>20.038733764899973</v>
       </c>
@@ -3115,7 +3115,7 @@
         <v>30.272243851199999</v>
       </c>
       <c r="N12" s="40"/>
-      <c r="O12" s="85"/>
+      <c r="O12" s="65"/>
     </row>
     <row r="13" spans="3:15" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C13" s="40"/>
@@ -3147,7 +3147,7 @@
         <v>21.996228436000003</v>
       </c>
       <c r="N13" s="40"/>
-      <c r="O13" s="85"/>
+      <c r="O13" s="65"/>
     </row>
     <row r="14" spans="3:15" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C14" s="40"/>
@@ -3179,7 +3179,7 @@
         <v>21.996228436000003</v>
       </c>
       <c r="N14" s="40"/>
-      <c r="O14" s="85"/>
+      <c r="O14" s="65"/>
     </row>
     <row r="15" spans="3:15" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C15" s="40"/>
@@ -3211,7 +3211,7 @@
         <v>21.996228436000003</v>
       </c>
       <c r="N15" s="40"/>
-      <c r="O15" s="85"/>
+      <c r="O15" s="65"/>
     </row>
     <row r="16" spans="3:15" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C16" s="40" t="s">
@@ -3247,7 +3247,7 @@
         <v>13.220697069000002</v>
       </c>
       <c r="N16" s="40"/>
-      <c r="O16" s="85"/>
+      <c r="O16" s="65"/>
     </row>
     <row r="17" spans="3:15" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C17" s="45">
@@ -3274,81 +3274,81 @@
         <f>93.14+48.78+21.22+16.73+6.25+3.89</f>
         <v>190.01</v>
       </c>
-      <c r="O17" s="86"/>
+      <c r="O17" s="66"/>
     </row>
     <row r="18" spans="3:15" x14ac:dyDescent="0.35">
-      <c r="C18" s="78" t="s">
+      <c r="C18" s="71" t="s">
         <v>50</v>
       </c>
-      <c r="D18" s="78"/>
-      <c r="E18" s="78"/>
-      <c r="F18" s="78"/>
-      <c r="G18" s="78"/>
+      <c r="D18" s="71"/>
+      <c r="E18" s="71"/>
+      <c r="F18" s="71"/>
+      <c r="G18" s="71"/>
       <c r="H18" s="37">
         <f>H11*3+O11*3</f>
         <v>1397.7352039346997</v>
       </c>
     </row>
     <row r="19" spans="3:15" x14ac:dyDescent="0.35">
-      <c r="C19" s="79" t="s">
+      <c r="C19" s="72" t="s">
         <v>51</v>
       </c>
-      <c r="D19" s="79"/>
-      <c r="E19" s="79"/>
-      <c r="F19" s="79"/>
-      <c r="G19" s="79"/>
+      <c r="D19" s="72"/>
+      <c r="E19" s="72"/>
+      <c r="F19" s="72"/>
+      <c r="G19" s="72"/>
       <c r="H19" s="37">
         <f>H18*0.75</f>
         <v>1048.3014029510248</v>
       </c>
     </row>
     <row r="20" spans="3:15" x14ac:dyDescent="0.35">
-      <c r="C20" s="79" t="s">
+      <c r="C20" s="72" t="s">
         <v>52</v>
       </c>
-      <c r="D20" s="79"/>
-      <c r="E20" s="79"/>
-      <c r="F20" s="79"/>
-      <c r="G20" s="79"/>
+      <c r="D20" s="72"/>
+      <c r="E20" s="72"/>
+      <c r="F20" s="72"/>
+      <c r="G20" s="72"/>
       <c r="H20" s="37">
         <f>H18*0.7</f>
         <v>978.41464275428973</v>
       </c>
     </row>
     <row r="21" spans="3:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="C21" s="77" t="s">
+      <c r="C21" s="67" t="s">
         <v>53</v>
       </c>
-      <c r="D21" s="77"/>
-      <c r="E21" s="77"/>
-      <c r="F21" s="77"/>
-      <c r="G21" s="77"/>
+      <c r="D21" s="67"/>
+      <c r="E21" s="67"/>
+      <c r="F21" s="67"/>
+      <c r="G21" s="67"/>
       <c r="H21" s="46">
         <f>SUM(H18:H20)</f>
         <v>3424.4512496400143</v>
       </c>
     </row>
     <row r="22" spans="3:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="C22" s="77" t="s">
+      <c r="C22" s="67" t="s">
         <v>54</v>
       </c>
-      <c r="D22" s="77"/>
-      <c r="E22" s="77"/>
-      <c r="F22" s="77"/>
-      <c r="G22" s="77"/>
+      <c r="D22" s="67"/>
+      <c r="E22" s="67"/>
+      <c r="F22" s="67"/>
+      <c r="G22" s="67"/>
       <c r="H22" s="46">
         <f>(H11*12)*0.85</f>
         <v>4547.9046089759986</v>
       </c>
     </row>
     <row r="23" spans="3:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="C23" s="77" t="s">
+      <c r="C23" s="67" t="s">
         <v>55</v>
       </c>
-      <c r="D23" s="77"/>
-      <c r="E23" s="77"/>
-      <c r="F23" s="77"/>
-      <c r="G23" s="77"/>
+      <c r="D23" s="67"/>
+      <c r="E23" s="67"/>
+      <c r="F23" s="67"/>
+      <c r="G23" s="67"/>
       <c r="H23" s="46">
         <f>H11*12</f>
         <v>5350.4760105599989</v>

</xml_diff>

<commit_message>
Actualizar precios desde Excel (test visual)
</commit_message>
<xml_diff>
--- a/src/PreciosP.xlsx
+++ b/src/PreciosP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro\calculadora-energia\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6BADEAC-BCC0-415D-9A0A-877F834A0D11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C03354B-4457-443A-9186-DA7E28F7BCD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{01D25416-3606-4CF3-ADEB-58FCB3C46A56}"/>
   </bookViews>
@@ -1506,22 +1506,22 @@
         <v>0.02</v>
       </c>
       <c r="J2" s="2">
-        <v>4.4200999999999997E-2</v>
+        <v>0.126775</v>
       </c>
       <c r="K2" s="2">
         <v>4.3700000000000003E-2</v>
       </c>
       <c r="L2" s="2">
         <f t="shared" ref="L2:L7" si="1">SUM(I2:K2)</f>
-        <v>0.107901</v>
+        <v>0.19047500000000001</v>
       </c>
       <c r="M2" s="2">
         <f t="shared" ref="M2:M7" si="2">L2*5%</f>
-        <v>5.3950500000000002E-3</v>
+        <v>9.523750000000001E-3</v>
       </c>
       <c r="N2" s="3">
         <f t="shared" ref="N2:N7" si="3">L2+M2</f>
-        <v>0.11329605</v>
+        <v>0.19999875</v>
       </c>
       <c r="Q2" s="33">
         <v>4.3700000000000003E-2</v>
@@ -1870,7 +1870,7 @@
       <c r="E11" s="40"/>
       <c r="F11" s="41">
         <f t="shared" ref="F11:F16" si="5">N2</f>
-        <v>0.11329605</v>
+        <v>0.19999875</v>
       </c>
       <c r="G11" s="43">
         <f t="shared" ref="G11:G16" si="6">E11*F11</f>

</xml_diff>